<commit_message>
need to test on other PC
</commit_message>
<xml_diff>
--- a/InitialResults/Graphs.xlsx
+++ b/InitialResults/Graphs.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni\Simulations\SwarmSimulation\InitialResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FC4597-DB6F-4A95-9B05-0591F60BAA59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5635E1-26AA-4134-9585-2BC38B98904B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13420" yWindow="1760" windowWidth="13520" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-7310" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Flow</t>
   </si>
@@ -37,6 +46,21 @@
   </si>
   <si>
     <t>Experimental results (From ali's paper_REF_)</t>
+  </si>
+  <si>
+    <t>MagTest2</t>
+  </si>
+  <si>
+    <t>MagTest3</t>
+  </si>
+  <si>
+    <t>ERR</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Experimental</t>
   </si>
 </sst>
 </file>
@@ -142,7 +166,7 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:marker>
             <c:symbol val="none"/>
@@ -270,12 +294,12 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000017-DC12-4B88-8EBB-F23622E824D0}"/>
+              <c16:uniqueId val="{0000000B-0FE3-4077-895F-4EE37C2A53C6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -382,7 +406,497 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000018-DC12-4B88-8EBB-F23622E824D0}"/>
+              <c16:uniqueId val="{0000000C-0FE3-4077-895F-4EE37C2A53C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>5216</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4705</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4205</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3457</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2805</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2161</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2111</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1705</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1266</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>955</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>259</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-0FE3-4077-895F-4EE37C2A53C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-0FE3-4077-895F-4EE37C2A53C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>5216</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4705</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4205</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3457</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2805</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2161</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2111</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1705</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1266</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>955</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>259</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-0FE3-4077-895F-4EE37C2A53C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-0FE3-4077-895F-4EE37C2A53C6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -852,20 +1366,1216 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$51:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$51:$B$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1086</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>981</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>767</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-2F23-4877-8B45-72AE0C6420C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$51:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$51:$C$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-2F23-4877-8B45-72AE0C6420C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$51:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$51:$B$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1086</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>981</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>767</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-2F23-4877-8B45-72AE0C6420C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$51:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$51:$C$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-2F23-4877-8B45-72AE0C6420C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="608128207"/>
+        <c:axId val="608129455"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="608128207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608129455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="608129455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608128207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>955</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>259</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F4F4-4082-91A4-7591090F1DC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$18:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F4F4-4082-91A4-7591090F1DC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="608128207"/>
+        <c:axId val="608129455"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="608128207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608129455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="608129455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608128207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$38:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$38:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1624</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1325</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1219</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-571B-4F13-B49E-359D4E133B52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$38:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$38:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-571B-4F13-B49E-359D4E133B52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="608128207"/>
+        <c:axId val="608129455"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="608128207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608129455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="608129455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608128207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>136525</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>87312</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>144462</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>441325</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>163512</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>339725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>30162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -923,6 +2633,120 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>244475</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96F8A6AA-A18F-4607-9B31-76135959691E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E70E8A6-856C-4245-83E9-E44E2F87C7F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21426D18-60DA-466B-B06A-7A2F9200D0A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1194,15 +3018,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:V58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1210,7 +3037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1E-3</v>
       </c>
@@ -1221,7 +3048,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1231,8 +3058,14 @@
       <c r="C3">
         <v>520</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="V3">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.01</v>
       </c>
@@ -1242,48 +3075,100 @@
       <c r="C4">
         <v>260</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>0.05</v>
+      </c>
+      <c r="V4">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V5">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>0.1</v>
+      </c>
+      <c r="V6">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="B8">
         <v>5216</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>0.15</v>
+      </c>
+      <c r="V8">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="B9">
         <v>4705</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.01</v>
       </c>
       <c r="B10">
         <v>4205</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>0.2</v>
+      </c>
+      <c r="V10">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="B11">
         <v>3654</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="V11">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.2E-2</v>
       </c>
@@ -1291,7 +3176,7 @@
         <v>3457</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1299,7 +3184,7 @@
         <v>2805</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -1307,7 +3192,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.02</v>
       </c>
@@ -1315,7 +3200,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1323,15 +3208,18 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="B17">
         <v>1266</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -1341,8 +3229,12 @@
       <c r="C18">
         <v>2000</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f>ABS((C18-B18)/C18)</f>
+        <v>0.52249999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.05</v>
       </c>
@@ -1352,8 +3244,12 @@
       <c r="C19">
         <v>1500</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" ref="D19:D24" si="0">ABS((C19-B19)/C19)</f>
+        <v>0.42666666666666669</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -1363,8 +3259,12 @@
       <c r="C20">
         <v>800</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.1</v>
       </c>
@@ -1374,8 +3274,12 @@
       <c r="C21">
         <v>650</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.2969230769230769</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.15</v>
       </c>
@@ -1385,8 +3289,12 @@
       <c r="C22">
         <v>500</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.2</v>
       </c>
@@ -1396,8 +3304,12 @@
       <c r="C23">
         <v>350</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.24571428571428572</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.22500000000000001</v>
       </c>
@@ -1407,77 +3319,229 @@
       <c r="C24">
         <v>250</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B26">
-        <v>1705</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>0.05</v>
-      </c>
-      <c r="B27">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="B28">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>0.1</v>
-      </c>
-      <c r="B29">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>0</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>0.15</v>
-      </c>
-      <c r="B31">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>0</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>0.2</v>
-      </c>
-      <c r="B33">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="B34">
-        <v>259</v>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f>SUM(D18:D24)/7</f>
+        <v>0.29897200418628989</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0.5</v>
+      </c>
+      <c r="B38">
+        <v>2265</v>
+      </c>
+      <c r="C38">
+        <v>1500</v>
+      </c>
+      <c r="D38">
+        <f>ABS((C38-B38)/C38)</f>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>1624</v>
+      </c>
+      <c r="C39">
+        <v>600</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ref="D39:D42" si="1">ABS((C39-B39)/C39)</f>
+        <v>1.7066666666666668</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1.5</v>
+      </c>
+      <c r="B40">
+        <v>1325</v>
+      </c>
+      <c r="C40">
+        <v>500</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1.75</v>
+      </c>
+      <c r="B41">
+        <v>1219</v>
+      </c>
+      <c r="C41">
+        <v>400</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>2.0474999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>1125</v>
+      </c>
+      <c r="C42">
+        <v>300</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f>SUM(D38:D42)/5</f>
+        <v>1.7328333333333332</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0.45</v>
+      </c>
+      <c r="B51">
+        <v>1602</v>
+      </c>
+      <c r="C51">
+        <v>2000</v>
+      </c>
+      <c r="D51">
+        <f>ABS((C51-B51)/C51)</f>
+        <v>0.19900000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0.5</v>
+      </c>
+      <c r="B52">
+        <v>1337</v>
+      </c>
+      <c r="C52">
+        <v>1500</v>
+      </c>
+      <c r="D52">
+        <f t="shared" ref="D52:D57" si="2">ABS((C52-B52)/C52)</f>
+        <v>0.10866666666666666</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0.75</v>
+      </c>
+      <c r="B53">
+        <v>1086</v>
+      </c>
+      <c r="C53">
+        <v>800</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>0.35749999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>981</v>
+      </c>
+      <c r="C54">
+        <v>650</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>0.50923076923076926</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1.5</v>
+      </c>
+      <c r="B55">
+        <v>810</v>
+      </c>
+      <c r="C55">
+        <v>500</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56">
+        <v>728</v>
+      </c>
+      <c r="C56">
+        <v>350</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2.25</v>
+      </c>
+      <c r="B57">
+        <v>767</v>
+      </c>
+      <c r="C57">
+        <v>250</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>2.0680000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <f>SUM(D51:D57)/7</f>
+        <v>0.70605677655677657</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test on other PC
</commit_message>
<xml_diff>
--- a/InitialResults/Graphs.xlsx
+++ b/InitialResults/Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni\Simulations\SwarmSimulation\InitialResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C01BBF-5511-4742-99BE-5D621723A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0872B4BF-E41C-4D9A-A025-F9517C4E1D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Flow</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>MagTest4</t>
+  </si>
+  <si>
+    <t>MagTest7</t>
+  </si>
+  <si>
+    <t>(MagTest6 in other graphs)</t>
+  </si>
+  <si>
+    <t>Velocity.*0.001</t>
   </si>
 </sst>
 </file>
@@ -3056,6 +3065,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2446</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1818</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1249</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1142</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1241</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3136,6 +3166,402 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D64D-4DC1-ACA7-930890D64826}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="608128207"/>
+        <c:axId val="608129455"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="608128207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Magnetic force (MA/m^2)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608129455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="608129455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time to travel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> 1mm (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608128207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$103:$A$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$103:$B$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1515</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1029</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>726</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6AE3-49E4-AC8B-D23FAC26F9D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$103:$A$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$103:$C$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6AE3-49E4-AC8B-D23FAC26F9D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3605,6 +4031,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3A321D1-A2BA-4979-B5B7-93B89438E555}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3871,10 +4335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V91"/>
+  <dimension ref="A1:V110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="O81" sqref="O81"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O83" sqref="O83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4540,90 +5004,246 @@
       <c r="A84">
         <v>0.45</v>
       </c>
+      <c r="B84">
+        <v>2446</v>
+      </c>
       <c r="C84">
         <v>2000</v>
       </c>
       <c r="D84">
         <f>ABS((C84-B84)/C84)</f>
-        <v>1</v>
+        <v>0.223</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0.5</v>
       </c>
+      <c r="B85">
+        <v>2220</v>
+      </c>
       <c r="C85">
         <v>1500</v>
       </c>
       <c r="D85">
         <f t="shared" ref="D85:D90" si="4">ABS((C85-B85)/C85)</f>
-        <v>1</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.75</v>
       </c>
+      <c r="B86">
+        <v>2009</v>
+      </c>
       <c r="C86">
         <v>800</v>
       </c>
       <c r="D86">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.51125</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1</v>
       </c>
+      <c r="B87">
+        <v>1818</v>
+      </c>
       <c r="C87">
         <v>650</v>
       </c>
       <c r="D87">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.7969230769230768</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1.5</v>
       </c>
+      <c r="B88">
+        <v>1249</v>
+      </c>
       <c r="C88">
         <v>500</v>
       </c>
       <c r="D88">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.498</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2</v>
       </c>
+      <c r="B89">
+        <v>1142</v>
+      </c>
       <c r="C89">
         <v>350</v>
       </c>
       <c r="D89">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2.2628571428571429</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2.25</v>
       </c>
+      <c r="B90">
+        <v>1241</v>
+      </c>
       <c r="C90">
         <v>250</v>
       </c>
       <c r="D90">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3.964</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D91">
         <f>SUM(D84:D90)/7</f>
+        <v>1.6765757456828887</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>0.45</v>
+      </c>
+      <c r="B103">
+        <v>1750</v>
+      </c>
+      <c r="C103">
+        <v>2000</v>
+      </c>
+      <c r="D103">
+        <f>ABS((C103-B103)/C103)</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>0.5</v>
+      </c>
+      <c r="B104">
+        <v>1515</v>
+      </c>
+      <c r="C104">
+        <v>1500</v>
+      </c>
+      <c r="D104">
+        <f t="shared" ref="D104:D109" si="5">ABS((C104-B104)/C104)</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>0.75</v>
+      </c>
+      <c r="B105">
+        <v>1122</v>
+      </c>
+      <c r="C105">
+        <v>800</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="5"/>
+        <v>0.40250000000000002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
         <v>1</v>
+      </c>
+      <c r="B106">
+        <v>1029</v>
+      </c>
+      <c r="C106">
+        <v>650</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="5"/>
+        <v>0.58307692307692305</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1.5</v>
+      </c>
+      <c r="B107">
+        <v>914</v>
+      </c>
+      <c r="C107">
+        <v>500</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="5"/>
+        <v>0.82799999999999996</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2</v>
+      </c>
+      <c r="B108">
+        <v>728</v>
+      </c>
+      <c r="C108">
+        <v>350</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="5"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2.25</v>
+      </c>
+      <c r="B109">
+        <v>726</v>
+      </c>
+      <c r="C109">
+        <v>250</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="5"/>
+        <v>1.9039999999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <f>SUM(D103:D109)/7</f>
+        <v>0.70465384615384608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes using wrong timeframe variables
</commit_message>
<xml_diff>
--- a/InitialResults/Graphs.xlsx
+++ b/InitialResults/Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni\Simulations\SwarmSimulation\InitialResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0872B4BF-E41C-4D9A-A025-F9517C4E1D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC2BD6B-00AC-4D0E-B84B-85E29FAC5503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Flow</t>
   </si>
@@ -77,6 +77,18 @@
   <si>
     <t>Velocity.*0.001</t>
   </si>
+  <si>
+    <t>MagTest8</t>
+  </si>
+  <si>
+    <t>Other PC</t>
+  </si>
+  <si>
+    <t>Velocity.*0.000001</t>
+  </si>
+  <si>
+    <t>Sizes:</t>
+  </si>
 </sst>
 </file>
 
@@ -111,8 +123,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3562,6 +3575,402 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6AE3-49E4-AC8B-D23FAC26F9D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="608128207"/>
+        <c:axId val="608129455"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="608128207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Magnetic force (MA/m^2)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608129455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="608129455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time to travel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> 1mm (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608128207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$123:$A$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$123:$B$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1659</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1528</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1322</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1064</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>759</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5F8A-4341-B126-C44BE5E2535A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$123:$A$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$123:$C$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5F8A-4341-B126-C44BE5E2535A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4069,6 +4478,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54DD5D78-C3E5-4AB3-8702-E22328D48AAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4335,10 +4782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V110"/>
+  <dimension ref="A1:V145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O83" sqref="O83"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="J143" sqref="J143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5246,6 +5693,154 @@
         <v>0.70465384615384608</v>
       </c>
     </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>14</v>
+      </c>
+      <c r="B122" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s">
+        <v>8</v>
+      </c>
+      <c r="D122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>0.45</v>
+      </c>
+      <c r="B123">
+        <v>1659</v>
+      </c>
+      <c r="C123">
+        <v>2000</v>
+      </c>
+      <c r="D123">
+        <f>ABS((C123-B123)/C123)</f>
+        <v>0.17050000000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>0.5</v>
+      </c>
+      <c r="B124">
+        <v>1528</v>
+      </c>
+      <c r="C124">
+        <v>1500</v>
+      </c>
+      <c r="D124">
+        <f t="shared" ref="D124:D129" si="6">ABS((C124-B124)/C124)</f>
+        <v>1.8666666666666668E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>0.75</v>
+      </c>
+      <c r="B125">
+        <v>1322</v>
+      </c>
+      <c r="C125">
+        <v>800</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="6"/>
+        <v>0.65249999999999997</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126">
+        <v>1064</v>
+      </c>
+      <c r="C126">
+        <v>650</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="6"/>
+        <v>0.63692307692307693</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>1.5</v>
+      </c>
+      <c r="B127">
+        <v>896</v>
+      </c>
+      <c r="C127">
+        <v>500</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="6"/>
+        <v>0.79200000000000004</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>2</v>
+      </c>
+      <c r="B128">
+        <v>767</v>
+      </c>
+      <c r="C128">
+        <v>350</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="6"/>
+        <v>1.1914285714285715</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>2.25</v>
+      </c>
+      <c r="B129">
+        <v>759</v>
+      </c>
+      <c r="C129">
+        <v>250</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="6"/>
+        <v>2.036</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <f>SUM(D123:D129)/7</f>
+        <v>0.78543118785975941</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
+        <v>17</v>
+      </c>
+      <c r="E144" s="1">
+        <v>4.4999999999999998E-14</v>
+      </c>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E145" s="1">
+        <v>4.7999999999999997E-12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changed to inner loop to ramp up force
</commit_message>
<xml_diff>
--- a/InitialResults/Graphs.xlsx
+++ b/InitialResults/Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni\Simulations\SwarmSimulation\InitialResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5AEBC9-61BF-4FCB-B706-CD3DB3E47AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD047E07-CE2A-4D9C-9DE7-EAD5F4198FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16290" yWindow="270" windowWidth="16395" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10065" yWindow="5775" windowWidth="25695" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t>Flow</t>
   </si>
@@ -122,6 +122,39 @@
   <si>
     <t>mention moving meeting to dfriday</t>
   </si>
+  <si>
+    <t>MagTest13 - x^-2 rateofchange cap</t>
+  </si>
+  <si>
+    <t>MagForce</t>
+  </si>
+  <si>
+    <t>ExpData</t>
+  </si>
+  <si>
+    <t>Different times obtained (no time maps saved)</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>MAX:</t>
+  </si>
+  <si>
+    <t>MIN:</t>
+  </si>
+  <si>
+    <t>AVG:</t>
+  </si>
+  <si>
+    <t>Error on that one point over 9 tests</t>
+  </si>
+  <si>
+    <t>MAGTEST14</t>
+  </si>
+  <si>
+    <t>rateofchange cap similarcap is less restrictive? No compound factor</t>
+  </si>
 </sst>
 </file>
 
@@ -144,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,13 +185,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3101,6 +3144,1121 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$252</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$253:$A$259</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$253:$B$259</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>889</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>893</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>795</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>592</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A6B4-4FCC-B2AD-838CA2024AB7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$252</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ExpData</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$253:$A$259</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$253:$C$259</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A6B4-4FCC-B2AD-838CA2024AB7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>0.45 Erro</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>0.45</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>0.45</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$265:$O$266</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>856</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A6B4-4FCC-B2AD-838CA2024AB7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>2.25 error</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>2.25</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2.25</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$265:$P$266</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>542</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A6B4-4FCC-B2AD-838CA2024AB7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>0.45 avg</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>0.45</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$267</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1058.7777777777778</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-A6B4-4FCC-B2AD-838CA2024AB7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>2.25 avg</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>2.25</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$267</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>622.11111111111109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-A6B4-4FCC-B2AD-838CA2024AB7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1192681775"/>
+        <c:axId val="1192682607"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1192681775"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1192682607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1192682607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1192681775"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$290</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$291:$A$297</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$291:$B$297</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="3">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>310</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9520-4A44-AA0D-D0BD6C655311}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$290</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ExpData</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$291:$A$297</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$291:$C$297</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9520-4A44-AA0D-D0BD6C655311}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1192700911"/>
+        <c:axId val="1192690927"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1192700911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1192690927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1192690927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1192700911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -6186,6 +7344,1118 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6720,6 +8990,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>519111</xdr:colOff>
+      <xdr:row>248</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DEF1F84-BDFF-42FD-9F3D-DC7FCE589665}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>304</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B203BE4B-E0F1-4F5B-B22F-C05A2F626845}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6986,10 +9328,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA239"/>
+  <dimension ref="A1:AA300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="A195" sqref="A195:A201"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="D294" sqref="D294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8750,6 +11092,405 @@
         <v>4.2181630036630029</v>
       </c>
     </row>
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>30</v>
+      </c>
+      <c r="B252" t="s">
+        <v>7</v>
+      </c>
+      <c r="C252" t="s">
+        <v>31</v>
+      </c>
+      <c r="O252" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>0.45</v>
+      </c>
+      <c r="B253">
+        <v>1192</v>
+      </c>
+      <c r="C253">
+        <v>2000</v>
+      </c>
+      <c r="D253">
+        <f t="shared" ref="D252:D256" si="14">ABS(C253-B253)/C253</f>
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="O253" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="P253" s="2">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>0.5</v>
+      </c>
+      <c r="B254">
+        <v>1050</v>
+      </c>
+      <c r="C254">
+        <v>1500</v>
+      </c>
+      <c r="D254">
+        <f t="shared" si="14"/>
+        <v>0.3</v>
+      </c>
+      <c r="O254">
+        <v>1130</v>
+      </c>
+      <c r="P254">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>0.75</v>
+      </c>
+      <c r="B255">
+        <v>889</v>
+      </c>
+      <c r="C255">
+        <v>800</v>
+      </c>
+      <c r="D255">
+        <f t="shared" si="14"/>
+        <v>0.11125</v>
+      </c>
+      <c r="O255">
+        <v>941</v>
+      </c>
+      <c r="P255">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>1</v>
+      </c>
+      <c r="B256">
+        <v>893</v>
+      </c>
+      <c r="C256">
+        <v>650</v>
+      </c>
+      <c r="D256">
+        <f t="shared" si="14"/>
+        <v>0.37384615384615383</v>
+      </c>
+      <c r="O256">
+        <v>1015</v>
+      </c>
+      <c r="P256">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>1.5</v>
+      </c>
+      <c r="B257">
+        <v>795</v>
+      </c>
+      <c r="C257">
+        <v>500</v>
+      </c>
+      <c r="D257">
+        <f>ABS(C257-B257)/C257</f>
+        <v>0.59</v>
+      </c>
+      <c r="O257">
+        <v>1112</v>
+      </c>
+      <c r="P257">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>2</v>
+      </c>
+      <c r="B258">
+        <v>643</v>
+      </c>
+      <c r="C258">
+        <v>350</v>
+      </c>
+      <c r="D258">
+        <f t="shared" ref="D258:D259" si="15">ABS(C258-B258)/C258</f>
+        <v>0.83714285714285719</v>
+      </c>
+      <c r="O258">
+        <v>1180</v>
+      </c>
+      <c r="P258">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>2.25</v>
+      </c>
+      <c r="B259">
+        <v>592</v>
+      </c>
+      <c r="C259">
+        <v>250</v>
+      </c>
+      <c r="D259">
+        <f t="shared" si="15"/>
+        <v>1.3680000000000001</v>
+      </c>
+      <c r="O259">
+        <v>1128</v>
+      </c>
+      <c r="P259" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D260">
+        <f>SUM(D257:D259)/3</f>
+        <v>0.93171428571428583</v>
+      </c>
+      <c r="O260">
+        <v>907</v>
+      </c>
+      <c r="P260">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D261">
+        <f>SUM(D253:D259)/7</f>
+        <v>0.56917700156985873</v>
+      </c>
+      <c r="O261">
+        <v>856</v>
+      </c>
+      <c r="P261">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D262">
+        <f>SUM(D253:D257)/5</f>
+        <v>0.35581923076923072</v>
+      </c>
+      <c r="O262">
+        <v>1260</v>
+      </c>
+      <c r="P262" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P263">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P264">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N265" t="s">
+        <v>34</v>
+      </c>
+      <c r="O265">
+        <f>MAX(O254:O262)</f>
+        <v>1260</v>
+      </c>
+      <c r="P265">
+        <f>MAX(P254:P264)</f>
+        <v>686</v>
+      </c>
+    </row>
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N266" t="s">
+        <v>35</v>
+      </c>
+      <c r="O266">
+        <f>MIN(O254:O262)</f>
+        <v>856</v>
+      </c>
+      <c r="P266">
+        <f>MIN(P254:P264)</f>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N267" t="s">
+        <v>36</v>
+      </c>
+      <c r="O267">
+        <f>AVERAGE(O254:O262)</f>
+        <v>1058.7777777777778</v>
+      </c>
+      <c r="P267">
+        <f>AVERAGE(P254:P264)</f>
+        <v>622.11111111111109</v>
+      </c>
+    </row>
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O269">
+        <f>(O265-O266)/O267</f>
+        <v>0.38157204323643612</v>
+      </c>
+      <c r="P269">
+        <f>(P265-P266)/P267</f>
+        <v>0.23146990534023934</v>
+      </c>
+    </row>
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O270" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>38</v>
+      </c>
+      <c r="B289" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>30</v>
+      </c>
+      <c r="B290" t="s">
+        <v>7</v>
+      </c>
+      <c r="C290" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>0.45</v>
+      </c>
+      <c r="C291">
+        <v>2000</v>
+      </c>
+      <c r="D291">
+        <f t="shared" ref="D291:D294" si="16">ABS(C291-B291)/C291</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>0.5</v>
+      </c>
+      <c r="C292">
+        <v>1500</v>
+      </c>
+      <c r="D292">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>0.75</v>
+      </c>
+      <c r="C293">
+        <v>800</v>
+      </c>
+      <c r="D293">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>1</v>
+      </c>
+      <c r="B294">
+        <v>575</v>
+      </c>
+      <c r="C294">
+        <v>650</v>
+      </c>
+      <c r="D294">
+        <f t="shared" si="16"/>
+        <v>0.11538461538461539</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>1.5</v>
+      </c>
+      <c r="B295">
+        <v>530</v>
+      </c>
+      <c r="C295">
+        <v>500</v>
+      </c>
+      <c r="D295">
+        <f>ABS(C295-B295)/C295</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>2</v>
+      </c>
+      <c r="B296">
+        <v>314</v>
+      </c>
+      <c r="C296">
+        <v>350</v>
+      </c>
+      <c r="D296">
+        <f t="shared" ref="D296:D297" si="17">ABS(C296-B296)/C296</f>
+        <v>0.10285714285714286</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>2.25</v>
+      </c>
+      <c r="B297">
+        <v>310</v>
+      </c>
+      <c r="C297">
+        <v>250</v>
+      </c>
+      <c r="D297">
+        <f t="shared" si="17"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D298">
+        <f>SUM(D295:D297)/3</f>
+        <v>0.13428571428571429</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D299">
+        <f>SUM(D291:D297)/7</f>
+        <v>0.50260596546310832</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D300">
+        <f>SUM(D291:D295)/5</f>
+        <v>0.63507692307692309</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
alter the times per second, think it works
</commit_message>
<xml_diff>
--- a/InitialResults/Graphs.xlsx
+++ b/InitialResults/Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni\Simulations\SwarmSimulation\InitialResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD047E07-CE2A-4D9C-9DE7-EAD5F4198FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3C617B-9FA1-4C7B-8695-52065DB2C582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10065" yWindow="5775" windowWidth="25695" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1665" yWindow="4110" windowWidth="28035" windowHeight="17130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>Flow</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>rateofchange cap similarcap is less restrictive? No compound factor</t>
+  </si>
+  <si>
+    <t>MAGTEST15</t>
   </si>
 </sst>
 </file>
@@ -4259,6 +4262,460 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$308</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$309:$A$315</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$309:$B$315</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7625999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1315999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59060000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.44900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.40200000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6BDA-4E2B-9F03-B6A543758A3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$308</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ExpData</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$309:$A$315</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$309:$C$315</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6BDA-4E2B-9F03-B6A543758A3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="46812143"/>
+        <c:axId val="46812559"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="46812143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="46812559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="46812559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="46812143"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -7387,6 +7844,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7943,6 +8440,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9062,6 +10075,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>442912</xdr:colOff>
+      <xdr:row>308</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>138112</xdr:colOff>
+      <xdr:row>322</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="18" name="Chart 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF9CDEEB-2AD6-4EF4-A70A-55CA3F4FC218}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9328,10 +10377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA300"/>
+  <dimension ref="A1:AA318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="D294" sqref="D294"/>
+    <sheetView tabSelected="1" topLeftCell="A295" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B308" sqref="B308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11122,7 +12171,7 @@
         <v>2000</v>
       </c>
       <c r="D253">
-        <f t="shared" ref="D252:D256" si="14">ABS(C253-B253)/C253</f>
+        <f t="shared" ref="D253:D256" si="14">ABS(C253-B253)/C253</f>
         <v>0.40400000000000003</v>
       </c>
       <c r="O253" s="2">
@@ -11489,6 +12538,145 @@
       <c r="D300">
         <f>SUM(D291:D295)/5</f>
         <v>0.63507692307692309</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>30</v>
+      </c>
+      <c r="B308" t="s">
+        <v>7</v>
+      </c>
+      <c r="C308" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>0.45</v>
+      </c>
+      <c r="B309">
+        <v>1.88</v>
+      </c>
+      <c r="C309">
+        <v>2</v>
+      </c>
+      <c r="D309">
+        <f t="shared" ref="D309:D312" si="18">ABS(C309-B309)/C309</f>
+        <v>6.0000000000000053E-2</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>0.5</v>
+      </c>
+      <c r="B310">
+        <v>1.7625999999999999</v>
+      </c>
+      <c r="C310">
+        <v>1.5</v>
+      </c>
+      <c r="D310">
+        <f>ABS(C310-B310)/C310</f>
+        <v>0.17506666666666662</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>0.75</v>
+      </c>
+      <c r="B311">
+        <v>1.1315999999999999</v>
+      </c>
+      <c r="C311">
+        <v>0.8</v>
+      </c>
+      <c r="D311">
+        <f>ABS(C311-B312)/C311</f>
+        <v>3.9999999999999897E-2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>1</v>
+      </c>
+      <c r="B312">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="C312">
+        <v>0.65</v>
+      </c>
+      <c r="D312">
+        <f>ABS(C312-B312)/C312</f>
+        <v>0.27999999999999992</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>1.5</v>
+      </c>
+      <c r="B313">
+        <v>0.59060000000000001</v>
+      </c>
+      <c r="C313">
+        <v>0.5</v>
+      </c>
+      <c r="D313">
+        <f>ABS(C313-B313)/C313</f>
+        <v>0.18120000000000003</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>2</v>
+      </c>
+      <c r="B314">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="C314">
+        <v>0.35</v>
+      </c>
+      <c r="D314">
+        <f t="shared" ref="D314:D315" si="19">ABS(C314-B314)/C314</f>
+        <v>0.28285714285714297</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>2.25</v>
+      </c>
+      <c r="B315">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="C315">
+        <v>0.25</v>
+      </c>
+      <c r="D315">
+        <f t="shared" si="19"/>
+        <v>0.6080000000000001</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D316">
+        <f>SUM(D313:D315)/3</f>
+        <v>0.35735238095238103</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D317">
+        <f>SUM(D309:D315)/7</f>
+        <v>0.23244625850340137</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D318">
+        <f>SUM(D309:D313)/5</f>
+        <v>0.14725333333333329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working version, 50x slower
</commit_message>
<xml_diff>
--- a/InitialResults/Graphs.xlsx
+++ b/InitialResults/Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni\Simulations\SwarmSimulation\InitialResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3C617B-9FA1-4C7B-8695-52065DB2C582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2E9A4A-0978-47B7-B4FE-951EDAC89F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="4110" windowWidth="28035" windowHeight="17130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16695" yWindow="3435" windowWidth="22650" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>Flow</t>
   </si>
@@ -158,6 +158,27 @@
   <si>
     <t>MAGTEST15</t>
   </si>
+  <si>
+    <t>MAGTEST17 - slowed down 50x</t>
+  </si>
+  <si>
+    <t>End Velocity</t>
+  </si>
+  <si>
+    <t>Time Graph</t>
+  </si>
+  <si>
+    <t>Velocity Graph</t>
+  </si>
+  <si>
+    <t>Last 3 results</t>
+  </si>
+  <si>
+    <t>Last 5 results</t>
+  </si>
+  <si>
+    <t>All 7</t>
+  </si>
 </sst>
 </file>
 
@@ -172,15 +193,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -197,14 +224,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4716,6 +4772,939 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$327</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$328:$A$334</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$328:$B$334</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.0095000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8890000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.50900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63049999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.29899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18275</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8929-468C-8CBE-CCFBEF351106}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$327</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ExpData</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$328:$A$334</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$328:$C$334</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8929-468C-8CBE-CCFBEF351106}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="814620191"/>
+        <c:axId val="814627679"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="814620191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="814627679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="814627679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="814620191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Time to travel 1mm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$346</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$347:$A$353</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$347:$B$353</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.8243</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5853999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0568</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79742999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.49349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36094999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32869999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0713-4371-94E3-A09AFCABBF14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$346</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ExpData</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$347:$A$353</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$347:$C$353</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0713-4371-94E3-A09AFCABBF14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="811405120"/>
+        <c:axId val="811396800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="811405120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="811396800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="811396800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="811405120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -5005,6 +5994,485 @@
     <c:showDLblsOverMax val="0"/>
     <c:extLst/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Velocity at 1mm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$346</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sim</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$347:$A$353</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$347:$F$353</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>9.728812436974792E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0269344537815124E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1861966638655463E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8638671260504201E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4313821176470598E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.017017058823532E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8175576722689086E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4E77-47E8-8412-8D9F3B495CD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$346</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ExpData</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$347:$A$353</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$347:$G$353</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.666666666666667E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.25E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5384615384615385E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8571428571428574E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4E77-47E8-8412-8D9F3B495CD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="811405120"/>
+        <c:axId val="811396800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="811405120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="811396800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="811396800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="811405120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -7923,6 +9391,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8956,6 +10544,1554 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10111,6 +13247,116 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>433387</xdr:colOff>
+      <xdr:row>325</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>339</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="19" name="Chart 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFB2DE68-141A-4636-8BC1-5C4AC279FD72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>345</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>359</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="20" name="Chart 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9152766A-979B-4FF0-8CDC-F24BB891969E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>345</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>360</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="21" name="Chart 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0E88C08-415E-4D39-98B4-51AA7A3741F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10377,15 +13623,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA318"/>
+  <dimension ref="A1:AA365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B308" sqref="B308"/>
+    <sheetView tabSelected="1" topLeftCell="A346" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B362" sqref="B362:D365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -12567,7 +15815,7 @@
         <v>2</v>
       </c>
       <c r="D309">
-        <f t="shared" ref="D309:D312" si="18">ABS(C309-B309)/C309</f>
+        <f t="shared" ref="D309" si="18">ABS(C309-B309)/C309</f>
         <v>6.0000000000000053E-2</v>
       </c>
     </row>
@@ -12677,6 +15925,447 @@
       <c r="D318">
         <f>SUM(D309:D313)/5</f>
         <v>0.14725333333333329</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>30</v>
+      </c>
+      <c r="B327" t="s">
+        <v>7</v>
+      </c>
+      <c r="C327" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>0.45</v>
+      </c>
+      <c r="B328">
+        <v>4.0095000000000001</v>
+      </c>
+      <c r="C328">
+        <v>2</v>
+      </c>
+      <c r="D328">
+        <f t="shared" ref="D328" si="20">ABS(C328-B328)/C328</f>
+        <v>1.00475</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>0.5</v>
+      </c>
+      <c r="B329">
+        <v>4.8890000000000002</v>
+      </c>
+      <c r="C329">
+        <v>1.5</v>
+      </c>
+      <c r="D329">
+        <f>ABS(C329-B329)/C329</f>
+        <v>2.2593333333333336</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>0.75</v>
+      </c>
+      <c r="B330">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="C330">
+        <v>0.8</v>
+      </c>
+      <c r="D330">
+        <f>ABS(C330-B331)/C330</f>
+        <v>0.21187500000000012</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>1</v>
+      </c>
+      <c r="B331">
+        <v>0.63049999999999995</v>
+      </c>
+      <c r="C331">
+        <v>0.65</v>
+      </c>
+      <c r="D331">
+        <f>ABS(C331-B331)/C331</f>
+        <v>3.000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>1.5</v>
+      </c>
+      <c r="B332">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="C332">
+        <v>0.5</v>
+      </c>
+      <c r="D332">
+        <f>ABS(C332-B332)/C332</f>
+        <v>0.40200000000000002</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>2</v>
+      </c>
+      <c r="B333">
+        <v>0.23849999999999999</v>
+      </c>
+      <c r="C333">
+        <v>0.35</v>
+      </c>
+      <c r="D333">
+        <f t="shared" ref="D333:D334" si="21">ABS(C333-B333)/C333</f>
+        <v>0.31857142857142856</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>2.25</v>
+      </c>
+      <c r="B334">
+        <v>0.18275</v>
+      </c>
+      <c r="C334">
+        <v>0.25</v>
+      </c>
+      <c r="D334">
+        <f t="shared" si="21"/>
+        <v>0.26900000000000002</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D335">
+        <f>SUM(D332:D334)/3</f>
+        <v>0.3298571428571429</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D336">
+        <f>SUM(D328:D334)/7</f>
+        <v>0.64221853741496615</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D337">
+        <f>SUM(D328:D332)/5</f>
+        <v>0.7815916666666668</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D338">
+        <f>SUM(D330:D334)/5</f>
+        <v>0.24628928571428571</v>
+      </c>
+    </row>
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>41</v>
+      </c>
+      <c r="D345" s="3"/>
+    </row>
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>30</v>
+      </c>
+      <c r="B346" t="s">
+        <v>7</v>
+      </c>
+      <c r="C346" t="s">
+        <v>31</v>
+      </c>
+      <c r="D346" s="3"/>
+      <c r="E346" t="s">
+        <v>42</v>
+      </c>
+      <c r="F346" t="s">
+        <v>7</v>
+      </c>
+      <c r="G346" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>0.45</v>
+      </c>
+      <c r="B347">
+        <v>1.8243</v>
+      </c>
+      <c r="C347">
+        <v>2</v>
+      </c>
+      <c r="D347" s="3">
+        <f t="shared" ref="D347:D353" si="22">ABS(C347-B347)/C347</f>
+        <v>8.7849999999999984E-2</v>
+      </c>
+      <c r="F347" s="1">
+        <v>9.728812436974792E-5</v>
+      </c>
+      <c r="G347">
+        <f>0.0001/C347</f>
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="H347" s="4">
+        <f>ABS(G347-F347)/G347</f>
+        <v>0.94576248739495827</v>
+      </c>
+    </row>
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>0.5</v>
+      </c>
+      <c r="B348">
+        <v>1.5853999999999999</v>
+      </c>
+      <c r="C348">
+        <v>1.5</v>
+      </c>
+      <c r="D348" s="3">
+        <f t="shared" si="22"/>
+        <v>5.693333333333328E-2</v>
+      </c>
+      <c r="F348">
+        <v>4.0269344537815124E-5</v>
+      </c>
+      <c r="G348">
+        <f t="shared" ref="G348:G353" si="23">0.0001/C348</f>
+        <v>6.666666666666667E-5</v>
+      </c>
+      <c r="H348" s="4">
+        <f t="shared" ref="H348:H353" si="24">ABS(G348-F348)/G348</f>
+        <v>0.39595983193277318</v>
+      </c>
+    </row>
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>0.75</v>
+      </c>
+      <c r="B349">
+        <v>1.0568</v>
+      </c>
+      <c r="C349">
+        <v>0.8</v>
+      </c>
+      <c r="D349" s="3">
+        <f t="shared" si="22"/>
+        <v>0.3209999999999999</v>
+      </c>
+      <c r="F349">
+        <v>1.1861966638655463E-4</v>
+      </c>
+      <c r="G349">
+        <f t="shared" si="23"/>
+        <v>1.25E-4</v>
+      </c>
+      <c r="H349" s="4">
+        <f t="shared" si="24"/>
+        <v>5.1042668907562969E-2</v>
+      </c>
+    </row>
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>1</v>
+      </c>
+      <c r="B350">
+        <v>0.79742999999999997</v>
+      </c>
+      <c r="C350">
+        <v>0.65</v>
+      </c>
+      <c r="D350" s="3">
+        <f t="shared" si="22"/>
+        <v>0.22681538461538453</v>
+      </c>
+      <c r="F350">
+        <v>1.8638671260504201E-4</v>
+      </c>
+      <c r="G350">
+        <f t="shared" si="23"/>
+        <v>1.5384615384615385E-4</v>
+      </c>
+      <c r="H350" s="4">
+        <f t="shared" si="24"/>
+        <v>0.21151363193277301</v>
+      </c>
+    </row>
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>1.5</v>
+      </c>
+      <c r="B351">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="C351">
+        <v>0.5</v>
+      </c>
+      <c r="D351" s="3">
+        <f t="shared" si="22"/>
+        <v>1.3000000000000012E-2</v>
+      </c>
+      <c r="F351">
+        <v>2.4313821176470598E-4</v>
+      </c>
+      <c r="G351">
+        <f t="shared" si="23"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="H351" s="4">
+        <f t="shared" si="24"/>
+        <v>0.21569105882352985</v>
+      </c>
+    </row>
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>2</v>
+      </c>
+      <c r="B352">
+        <v>0.36094999999999999</v>
+      </c>
+      <c r="C352">
+        <v>0.35</v>
+      </c>
+      <c r="D352" s="3">
+        <f t="shared" si="22"/>
+        <v>3.1285714285714333E-2</v>
+      </c>
+      <c r="F352">
+        <v>3.017017058823532E-4</v>
+      </c>
+      <c r="G352">
+        <f t="shared" si="23"/>
+        <v>2.8571428571428574E-4</v>
+      </c>
+      <c r="H352" s="4">
+        <f t="shared" si="24"/>
+        <v>5.5955970588236106E-2</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>2.25</v>
+      </c>
+      <c r="B353">
+        <v>0.32869999999999999</v>
+      </c>
+      <c r="C353">
+        <v>0.25</v>
+      </c>
+      <c r="D353" s="3">
+        <f t="shared" si="22"/>
+        <v>0.31479999999999997</v>
+      </c>
+      <c r="F353">
+        <v>3.8175576722689086E-4</v>
+      </c>
+      <c r="G353">
+        <f t="shared" si="23"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="H353" s="4">
+        <f t="shared" si="24"/>
+        <v>4.5610581932772898E-2</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D354" s="3">
+        <f>SUM(D351:D353)/3</f>
+        <v>0.11969523809523812</v>
+      </c>
+      <c r="H354" s="4">
+        <f>SUM(H351:H353)/3</f>
+        <v>0.10575253711484628</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D355" s="3">
+        <f>SUM(D347:D353)/7</f>
+        <v>0.15024063317634745</v>
+      </c>
+      <c r="H355" s="3">
+        <f>SUM(H347:H353)/7</f>
+        <v>0.27450517593037238</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D356" s="3">
+        <f>SUM(D347:D351)/5</f>
+        <v>0.14111974358974352</v>
+      </c>
+      <c r="H356" s="4">
+        <f>SUM(H347:H351)/5</f>
+        <v>0.36399393579831946</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D357" s="3">
+        <f>SUM(D349:D353)/5</f>
+        <v>0.18138021978021973</v>
+      </c>
+      <c r="H357" s="4">
+        <f>SUM(H349:H353)/5</f>
+        <v>0.11596278243697497</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H361">
+        <v>0.10575253711484628</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B362" s="7"/>
+      <c r="C362" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D362" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B363" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C363" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="D363" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B364" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C364" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="D364" s="6">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B365" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C365" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D365" s="6">
+        <v>0.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>